<commit_message>
updated resource metadata mapping
</commit_message>
<xml_diff>
--- a/data-raw/constant_vocab_mapping.xlsx
+++ b/data-raw/constant_vocab_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB525812\cmder\Git Repos\eex2ddh\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786A7A77-5C65-444D-9FA1-E55D42E9E9CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35505C73-86B8-4954-9E6A-F9D94E164454}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>is_dataset</t>
   </si>
@@ -947,10 +947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,7 +1128,19 @@
         <v>0</v>
       </c>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added people soft ids for ttl and collaborators
</commit_message>
<xml_diff>
--- a/data-raw/constant_vocab_mapping.xlsx
+++ b/data-raw/constant_vocab_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB525812\cmder\Git Repos\eex2ddh\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35505C73-86B8-4954-9E6A-F9D94E164454}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B98A29E-225C-4F1B-AB43-284F0DEB0D49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,9 +76,6 @@
     <t>field_wbddh_ds_source</t>
   </si>
   <si>
-    <t>458070, 530865</t>
-  </si>
-  <si>
     <t>field_wbddh_collaborator_upi</t>
   </si>
   <si>
@@ -107,6 +104,9 @@
   </si>
   <si>
     <t>eex_value</t>
+  </si>
+  <si>
+    <t>23715, 54524</t>
   </si>
 </sst>
 </file>
@@ -950,7 +950,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,13 +962,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" t="s">
-        <v>28</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1012,7 +1012,7 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>336592</v>
+        <v>15062</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
@@ -1075,10 +1075,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
@@ -1086,10 +1086,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
@@ -1097,10 +1097,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -1108,10 +1108,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
added og_group_ref for collections
</commit_message>
<xml_diff>
--- a/data-raw/constant_vocab_mapping.xlsx
+++ b/data-raw/constant_vocab_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB525812\cmder\Git Repos\eex2ddh\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B98A29E-225C-4F1B-AB43-284F0DEB0D49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE6AFC9-5521-4103-BC56-D1AC6738F226}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>is_dataset</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>23715, 54524</t>
+  </si>
+  <si>
+    <t>og_group_ref</t>
   </si>
 </sst>
 </file>
@@ -947,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,6 +1142,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17">
+        <v>144795</v>
+      </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
made changes for collection feature
</commit_message>
<xml_diff>
--- a/data-raw/constant_vocab_mapping.xlsx
+++ b/data-raw/constant_vocab_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB525812\cmder\Git Repos\eex2ddh\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE6AFC9-5521-4103-BC56-D1AC6738F226}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05A9006-5AE0-4C93-AE2D-1956AD27C1EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,7 +109,7 @@
     <t>23715, 54524</t>
   </si>
   <si>
-    <t>og_group_ref</t>
+    <t>field_collection_field</t>
   </si>
 </sst>
 </file>
@@ -953,7 +953,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,7 +1147,7 @@
         <v>29</v>
       </c>
       <c r="B17">
-        <v>144795</v>
+        <v>1566</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
quick change for taxonomy value
</commit_message>
<xml_diff>
--- a/data-raw/constant_vocab_mapping.xlsx
+++ b/data-raw/constant_vocab_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB525812\cmder\Git Repos\eex2ddh\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05A9006-5AE0-4C93-AE2D-1956AD27C1EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A769920-A862-4874-89F6-BB5A2663B6C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>is_dataset</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>field_collection_field</t>
+  </si>
+  <si>
+    <t>ENERGY DATA.INFO</t>
   </si>
 </sst>
 </file>
@@ -1146,8 +1149,8 @@
       <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="B17">
-        <v>1566</v>
+      <c r="B17" t="s">
+        <v>30</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
made changes for Jemi and Shandao leaving, and updated Tigran UPI
</commit_message>
<xml_diff>
--- a/data-raw/constant_vocab_mapping.xlsx
+++ b/data-raw/constant_vocab_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB525812\cmder\Git Repos\eex2ddh\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A769920-A862-4874-89F6-BB5A2663B6C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7342E838-7DD5-4319-86DE-75A41D7014CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>is_dataset</t>
   </si>
@@ -104,9 +104,6 @@
   </si>
   <si>
     <t>eex_value</t>
-  </si>
-  <si>
-    <t>23715, 54524</t>
   </si>
   <si>
     <t>field_collection_field</t>
@@ -255,7 +252,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -433,6 +430,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -596,8 +599,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -956,7 +960,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,14 +1017,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>15062</v>
-      </c>
-      <c r="D5" t="b">
+      <c r="B5" s="1">
+        <v>336592</v>
+      </c>
+      <c r="D5" s="1" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1079,14 +1083,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" t="b">
+      <c r="B11" s="1">
+        <v>511294</v>
+      </c>
+      <c r="D11" s="1" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1147,10 +1151,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
         <v>29</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>

</xml_diff>